<commit_message>
updated trend analysis functions to work with new spread sheet format using subject/action words, updated test script accordingly
</commit_message>
<xml_diff>
--- a/output data/hazard_interpretation_test.xlsx
+++ b/output data/hazard_interpretation_test.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24026"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\srandrad\smart_nlp\output data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5ADF54D5-B77E-4392-90FC-806D62F9C745}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B13B4B8-8085-4468-8C3B-E194A5C6C7AD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14016" xr2:uid="{1E09127A-9D7A-4A65-B2FF-C060090E7D3B}"/>
+    <workbookView xWindow="1848" yWindow="1848" windowWidth="17280" windowHeight="10044" xr2:uid="{1E09127A-9D7A-4A65-B2FF-C060090E7D3B}"/>
   </bookViews>
   <sheets>
     <sheet name="Hazard-focused" sheetId="1" r:id="rId1"/>
@@ -35,10 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="21">
-  <si>
-    <t>Hazard words</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="25">
   <si>
     <t>Hazard level 1 topics</t>
   </si>
@@ -88,16 +85,31 @@
     <t>Traffic Hazard</t>
   </si>
   <si>
-    <t>highway, road; close, closure</t>
-  </si>
-  <si>
-    <t>ground; aircraft, helicopter, heli, copter, aerial, tanker</t>
-  </si>
-  <si>
     <t>Aerial Grounding</t>
   </si>
   <si>
-    <t>resource, crew; limited, share, lack, fatigue</t>
+    <t>Hazard Noun/Subject</t>
+  </si>
+  <si>
+    <t>Action/Descriptor</t>
+  </si>
+  <si>
+    <t>resource, crew</t>
+  </si>
+  <si>
+    <t>limited, share, lack, fatigue</t>
+  </si>
+  <si>
+    <t>highway, road</t>
+  </si>
+  <si>
+    <t>close, closure</t>
+  </si>
+  <si>
+    <t>ground</t>
+  </si>
+  <si>
+    <t>aircraft, helicopter, heli, copter, aerial, tanker</t>
   </si>
 </sst>
 </file>
@@ -461,70 +473,81 @@
   <dimension ref="A1:M4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="J13" sqref="J13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>0</v>
-      </c>
-      <c r="B1" s="1"/>
-      <c r="C1" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>1</v>
       </c>
       <c r="F1" s="1"/>
       <c r="G1" s="1" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H1" s="1"/>
       <c r="I1" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="J1" s="1"/>
       <c r="K1" s="1" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="L1" s="1"/>
       <c r="M1" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B2" t="s">
         <v>20</v>
       </c>
       <c r="K2" t="s">
+        <v>12</v>
+      </c>
+      <c r="M2" t="s">
         <v>13</v>
-      </c>
-      <c r="M2" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>17</v>
+        <v>21</v>
+      </c>
+      <c r="B3" t="s">
+        <v>22</v>
       </c>
       <c r="K3" t="s">
+        <v>14</v>
+      </c>
+      <c r="M3" t="s">
         <v>15</v>
-      </c>
-      <c r="M3" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>18</v>
+        <v>23</v>
+      </c>
+      <c r="B4" t="s">
+        <v>24</v>
       </c>
       <c r="K4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="M4" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
     </row>
   </sheetData>
@@ -545,29 +568,29 @@
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B1" s="1"/>
       <c r="C1" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D1" s="1"/>
       <c r="E1" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F1" s="1"/>
       <c r="G1" s="1"/>
       <c r="H1" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="I1" s="1"/>
       <c r="J1" s="1"/>
       <c r="K1" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="L1" s="1"/>
       <c r="M1" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>